<commit_message>
Improving bulk booking data parsing
</commit_message>
<xml_diff>
--- a/backend/shipping/data/failure.xlsx
+++ b/backend/shipping/data/failure.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Row No</t>
   </si>
@@ -21,6 +21,12 @@
   </si>
   <si>
     <t>Error Message</t>
+  </si>
+  <si>
+    <t>CR940111</t>
+  </si>
+  <si>
+    <t>Object reference not set to an instance of an object.</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -82,6 +88,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
improved to book a waybill thru waybill sheet
</commit_message>
<xml_diff>
--- a/backend/shipping/data/failure.xlsx
+++ b/backend/shipping/data/failure.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Row No</t>
   </si>
@@ -21,12 +21,6 @@
   </si>
   <si>
     <t>Error Message</t>
-  </si>
-  <si>
-    <t>CR940111</t>
-  </si>
-  <si>
-    <t>Object reference not set to an instance of an object.</t>
   </si>
 </sst>
 </file>
@@ -71,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,17 +82,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
imroved bulk upload with itemdetails sucess generation
</commit_message>
<xml_diff>
--- a/backend/shipping/data/failure.xlsx
+++ b/backend/shipping/data/failure.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Row No</t>
   </si>
@@ -21,12 +21,6 @@
   </si>
   <si>
     <t>Error Message</t>
-  </si>
-  <si>
-    <t>CR940125</t>
-  </si>
-  <si>
-    <t>Bluedart rejected the request</t>
   </si>
 </sst>
 </file>
@@ -71,7 +65,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,17 +82,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>